<commit_message>
update latex report with deep learning material
</commit_message>
<xml_diff>
--- a/NN Project 2/results.xlsx
+++ b/NN Project 2/results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11203"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/npatel/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/npatel/Library/CloudStorage/Dropbox/Nish/Rutgers MSDS/3_2023F/Massive Data Storage/Project/Rutgers-CS543-Group4-AML/NN Project 2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{41CF2F53-12C9-A743-AF29-4519509A0278}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75F03767-F212-9948-A2E2-8EB0CA94168C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1140" yWindow="500" windowWidth="50100" windowHeight="28300" xr2:uid="{490D8B28-406F-B847-BAD5-1E415AB41F1C}"/>
+    <workbookView xWindow="1100" yWindow="500" windowWidth="50100" windowHeight="28300" xr2:uid="{490D8B28-406F-B847-BAD5-1E415AB41F1C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -191,6 +191,55 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>128588</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>126206</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CE22E56F-FF8F-5797-EC3D-94ABE97DF13F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8691563" y="3714750"/>
+          <a:ext cx="7772400" cy="1983581"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -513,7 +562,7 @@
   <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -953,5 +1002,6 @@
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>